<commit_message>
Add Preston's hours from project discussion meetings
</commit_message>
<xml_diff>
--- a/project-management/time-tracking.xlsx
+++ b/project-management/time-tracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prest\Documents\Preston\School\University of Cincinnati\Semester 7 (Fall 2024)\CS 5001 - Senior Design I\senior-design\project-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3B9792-8B16-4EE9-ABEC-D323AB503186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E6AD44-6AF9-4024-A750-7C89F5159EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preston" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>Date:</t>
   </si>
@@ -51,6 +51,18 @@
   </si>
   <si>
     <t>Running total:</t>
+  </si>
+  <si>
+    <t>Initial team meeting, discussed project and advisor ideas</t>
+  </si>
+  <si>
+    <t>Met with Dr. Gallagher to discuss Neromorphic Constraint Satisfaction project, and discussed with team</t>
+  </si>
+  <si>
+    <t>Met with Jeremy Hill to discuss TA scheduling software (generally, scheduling with constraints)</t>
+  </si>
+  <si>
+    <t>Met with Dr. Abuaitah to discuss assembly code simulator/educational tool project, and discussed with team</t>
   </si>
 </sst>
 </file>
@@ -96,13 +108,13 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -391,17 +403,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="13.3125" style="2" customWidth="1"/>
     <col min="2" max="2" width="8.83984375" style="1"/>
-    <col min="3" max="3" width="55.05078125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="85.9453125" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.83984375" style="1"/>
     <col min="5" max="5" width="15.3125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.83984375" style="1"/>
@@ -419,15 +431,54 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="5"/>
+      <c r="A2" s="5">
+        <v>45531</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="5">
+        <v>45532</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="5">
+        <v>45533</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="3">
         <f>SUM(B2:B1000)</f>
-        <v>0</v>
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="5">
+        <v>45533</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -531,7 +582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C4AD561-4D49-4B54-ACF1-10A35B54733B}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add hours for week of 9/9
</commit_message>
<xml_diff>
--- a/project-management/time-tracking.xlsx
+++ b/project-management/time-tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prest\Documents\Preston\School\University of Cincinnati\Semester 7 (Fall 2024)\CS 5001 - Senior Design I\senior-design\project-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E6AD44-6AF9-4024-A750-7C89F5159EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F28092-9D17-4E30-A3A9-2B0018156867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
   <si>
     <t>Date:</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>Met with Dr. Abuaitah to discuss assembly code simulator/educational tool project, and discussed with team</t>
+  </si>
+  <si>
+    <t>Met with Dr. Abuaitah to discuss project logistics and expectations</t>
+  </si>
+  <si>
+    <t>Met with team to draft contract and decide roles</t>
   </si>
 </sst>
 </file>
@@ -403,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -467,7 +473,7 @@
       </c>
       <c r="F4" s="3">
         <f>SUM(B2:B1000)</f>
-        <v>3.25</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -479,6 +485,28 @@
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="5">
+        <v>45545</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="5">
+        <v>45545</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add hours for weeks of 9-9 and 9-16
</commit_message>
<xml_diff>
--- a/project-management/time-tracking.xlsx
+++ b/project-management/time-tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prest\Documents\Preston\School\University of Cincinnati\Semester 7 (Fall 2024)\CS 5001 - Senior Design I\senior-design\project-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F28092-9D17-4E30-A3A9-2B0018156867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5C7DDE-F8BE-484E-8312-0146DD2E5C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>Date:</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>Met with team to draft contract and decide roles</t>
+  </si>
+  <si>
+    <t>Individual Capstone Assessment</t>
+  </si>
+  <si>
+    <t>Access and clone Hacademia repository</t>
+  </si>
+  <si>
+    <t>Review design diagram examples</t>
+  </si>
+  <si>
+    <t>Write user stories and create design diagrams</t>
   </si>
 </sst>
 </file>
@@ -409,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -473,7 +485,7 @@
       </c>
       <c r="F4" s="3">
         <f>SUM(B2:B1000)</f>
-        <v>4.5</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -507,6 +519,61 @@
       </c>
       <c r="C7" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="5">
+        <v>45547</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="5">
+        <v>45549</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="5">
+        <v>45550</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="5">
+        <v>45551</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="5">
+        <v>45552</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add weekly meeting 9-24
</commit_message>
<xml_diff>
--- a/project-management/time-tracking.xlsx
+++ b/project-management/time-tracking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prest\Documents\Preston\School\University of Cincinnati\Semester 7 (Fall 2024)\CS 5001 - Senior Design I\senior-design\project-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5C7DDE-F8BE-484E-8312-0146DD2E5C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEB464B-7E7B-47F2-84BC-CE7480F740BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>Date:</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Write user stories and create design diagrams</t>
+  </si>
+  <si>
+    <t>Develop task lists</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -485,7 +488,7 @@
       </c>
       <c r="F4" s="3">
         <f>SUM(B2:B1000)</f>
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -574,6 +577,17 @@
       </c>
       <c r="C12" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="5">
+        <v>45559</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>